<commit_message>
Gestion de risques updatée
</commit_message>
<xml_diff>
--- a/Gestion/Gestion de risques.xlsx
+++ b/Gestion/Gestion de risques.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederic\Google Drive\Génie Électrique\S5\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederic\Desktop\ProjetS5\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="6630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="6630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Risques fonctionnels" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Risques de gestion'!$A$2:$G$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Risques fonctionnels'!$A$2:$I$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Risques humains'!$A$2:$G$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Risques fonctionnels'!$A$2:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Risques humains'!$A$2:$H$9</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
   <si>
     <t>Risque</t>
   </si>
@@ -320,6 +320,39 @@
   </si>
   <si>
     <t>Se rapporter au barême à chaque semaine</t>
+  </si>
+  <si>
+    <t>Code d'assurance-qualité</t>
+  </si>
+  <si>
+    <t>3.T.1</t>
+  </si>
+  <si>
+    <t>2.T.2</t>
+  </si>
+  <si>
+    <t>2.T</t>
+  </si>
+  <si>
+    <t>2.T.2.1</t>
+  </si>
+  <si>
+    <t>2.T.2.2</t>
+  </si>
+  <si>
+    <t>1.T.2.3</t>
+  </si>
+  <si>
+    <t>1.T.2.2</t>
+  </si>
+  <si>
+    <t>2.T.1.4</t>
+  </si>
+  <si>
+    <t>1.T.3.1</t>
+  </si>
+  <si>
+    <t>1.T.1.2</t>
   </si>
 </sst>
 </file>
@@ -467,6 +500,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -502,6 +552,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -654,24 +721,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31.265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.06640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="10.6640625" style="1"/>
-    <col min="8" max="8" width="44.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="44.46484375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="23.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.06640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="10.6640625" style="1"/>
+    <col min="9" max="9" width="44.73046875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.46484375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -683,294 +751,325 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
       <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
-        <v>3</v>
-      </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G12" si="0">D3*E3*F3</f>
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H12" si="0">E3*F3*G3</f>
         <v>45</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1">
-        <v>2</v>
+      <c r="B4" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
         <v>5</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>4</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
-        <v>2</v>
+      <c r="B5" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
         <v>5</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
       <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
       <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
       <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
       <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
       <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="1">
-        <v>2</v>
-      </c>
       <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
       <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="1">
-        <v>2</v>
-      </c>
       <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
         <v>5</v>
       </c>
-      <c r="F9" s="1">
-        <v>3</v>
-      </c>
       <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1">
-        <v>3</v>
+      <c r="B10" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="1">
-        <v>3</v>
-      </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1">
-        <v>2</v>
+      <c r="B12" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -979,26 +1078,29 @@
         <v>2</v>
       </c>
       <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I12">
-    <sortState ref="A3:I12">
-      <sortCondition descending="1" ref="G2:G12"/>
+  <autoFilter ref="A2:J12">
+    <sortState ref="A3:J12">
+      <sortCondition descending="1" ref="H2:H12"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G3:G12">
+  <conditionalFormatting sqref="H3:H12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1017,22 +1119,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31.265625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="10.6640625" style="1"/>
-    <col min="6" max="6" width="44.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.46484375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.6640625" style="1"/>
+    <col min="7" max="7" width="44.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.46484375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1042,157 +1145,158 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>4</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E9" si="0">B3*C3*D3</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F9" si="0">C3*D3*E3</f>
         <v>48</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
       </c>
       <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
         <v>5</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -1200,50 +1304,53 @@
         <v>2</v>
       </c>
       <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G9">
-    <sortState ref="A3:G9">
-      <sortCondition descending="1" ref="E2:E9"/>
+  <autoFilter ref="A2:H9">
+    <sortState ref="A3:H9">
+      <sortCondition descending="1" ref="F2:F9"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E9">
+  <conditionalFormatting sqref="F3:F9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1263,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>